<commit_message>
Updated Excel, Added Mail Part, Encrypted Personal Data
</commit_message>
<xml_diff>
--- a/Configuration/Config.xlsx
+++ b/Configuration/Config.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20395"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav\Documents\UiPath\Wikipedia_Automation\Configuration\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF60000-1119-4BFF-B5C4-418FEC030818}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Static" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -23,34 +29,96 @@
     <t>Value</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/w/index.php?title=A._P._J._Abdul_Kalam&amp;action=history</t>
+  </si>
+  <si>
+    <t>URL to work</t>
+  </si>
+  <si>
+    <t>Prefered_Size</t>
+  </si>
+  <si>
+    <t>Provide the value in bytes</t>
+  </si>
+  <si>
     <t>Name_Change</t>
   </si>
   <si>
+    <t>20:00, 18 March 2023</t>
+  </si>
+  <si>
     <t>Size_Change</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/w/index.php?title=A._P._J._Abdul_Kalam&amp;action=history</t>
-  </si>
-  <si>
-    <t>URL to work</t>
-  </si>
-  <si>
-    <t>Prefered_Size</t>
-  </si>
-  <si>
-    <t>Provide the value in bytes</t>
+    <t>144,909 bytes</t>
+  </si>
+  <si>
+    <t>Mail Body</t>
+  </si>
+  <si>
+    <t>Mail Subject</t>
+  </si>
+  <si>
+    <t>What you want to write in mail body</t>
+  </si>
+  <si>
+    <t>Subject of Mail</t>
+  </si>
+  <si>
+    <t>Hi Sir,
+There are large changes on Website
+Sent From Bot</t>
+  </si>
+  <si>
+    <t>Major Changes on Site</t>
+  </si>
+  <si>
+    <t>Send To</t>
+  </si>
+  <si>
+    <t>Send CC</t>
+  </si>
+  <si>
+    <t>Email Ids for cc Part</t>
+  </si>
+  <si>
+    <t>Send From</t>
+  </si>
+  <si>
+    <t>From which email Id need to send mail</t>
+  </si>
+  <si>
+    <t>Enter multiple email id in comma seperated form</t>
+  </si>
+  <si>
+    <t>gauravkeny1@gmail.com</t>
+  </si>
+  <si>
+    <t>lRMNNqzor31QjVFoWEm+oI5JpLHDEhVBNROJe2hWdd6saS2fitYM2zAL19uO5Hv9Uum30eANlraiO/P+Gkv9hxcawzQ8oWdHZFb9xwK0y6rKgexShlbQEWkk3/ZgBahb+JC2dMuHmnVJKqqeFA==</t>
+  </si>
+  <si>
+    <t>Encrypted Client ID</t>
+  </si>
+  <si>
+    <t>Enc Client ID</t>
+  </si>
+  <si>
+    <t>S+Rq0hUcXnUAFSA47AfGpKVU9uhkW1PFMwlM/cpzHvN6yCYdplU8L1f6xnBGyWmsQHXlZ0mu7+Us6M0zuNJiEi42xT1kuDE=</t>
+  </si>
+  <si>
+    <t>Enc Client Secret</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -80,9 +148,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -94,6 +171,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -142,7 +222,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,9 +255,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -210,6 +307,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -385,51 +499,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="76.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" s="2">
+        <v>500</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1">
-        <v>500</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
+    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -438,16 +627,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:A26"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -460,12 +650,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some issues in selector just updated it.
</commit_message>
<xml_diff>
--- a/Configuration/Config.xlsx
+++ b/Configuration/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav\Documents\UiPath\Wikipedia_Automation\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF60000-1119-4BFF-B5C4-418FEC030818}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8C31BA-EF0E-4250-A730-CF1AB9E2FBD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -32,6 +32,9 @@
     <t>Description</t>
   </si>
   <si>
+    <t>SITE UPDATES</t>
+  </si>
+  <si>
     <t>URL</t>
   </si>
   <si>
@@ -47,28 +50,10 @@
     <t>Provide the value in bytes</t>
   </si>
   <si>
-    <t>Name_Change</t>
-  </si>
-  <si>
-    <t>20:00, 18 March 2023</t>
-  </si>
-  <si>
-    <t>Size_Change</t>
-  </si>
-  <si>
-    <t>144,909 bytes</t>
+    <t>MAILS UPDATES</t>
   </si>
   <si>
     <t>Mail Body</t>
-  </si>
-  <si>
-    <t>Mail Subject</t>
-  </si>
-  <si>
-    <t>What you want to write in mail body</t>
-  </si>
-  <si>
-    <t>Subject of Mail</t>
   </si>
   <si>
     <t>Hi Sir,
@@ -76,12 +61,27 @@
 Sent From Bot</t>
   </si>
   <si>
+    <t>What you want to write in mail body</t>
+  </si>
+  <si>
+    <t>Mail Subject</t>
+  </si>
+  <si>
     <t>Major Changes on Site</t>
   </si>
   <si>
+    <t>Subject of Mail</t>
+  </si>
+  <si>
     <t>Send To</t>
   </si>
   <si>
+    <t>gauravkeny1@gmail.com</t>
+  </si>
+  <si>
+    <t>Enter multiple email id in comma seperated form</t>
+  </si>
+  <si>
     <t>Send CC</t>
   </si>
   <si>
@@ -94,10 +94,7 @@
     <t>From which email Id need to send mail</t>
   </si>
   <si>
-    <t>Enter multiple email id in comma seperated form</t>
-  </si>
-  <si>
-    <t>gauravkeny1@gmail.com</t>
+    <t>Enc Client ID</t>
   </si>
   <si>
     <t>lRMNNqzor31QjVFoWEm+oI5JpLHDEhVBNROJe2hWdd6saS2fitYM2zAL19uO5Hv9Uum30eANlraiO/P+Gkv9hxcawzQ8oWdHZFb9xwK0y6rKgexShlbQEWkk3/ZgBahb+JC2dMuHmnVJKqqeFA==</t>
@@ -106,13 +103,61 @@
     <t>Encrypted Client ID</t>
   </si>
   <si>
-    <t>Enc Client ID</t>
+    <t>Enc Client Secret</t>
   </si>
   <si>
     <t>S+Rq0hUcXnUAFSA47AfGpKVU9uhkW1PFMwlM/cpzHvN6yCYdplU8L1f6xnBGyWmsQHXlZ0mu7+Us6M0zuNJiEi42xT1kuDE=</t>
   </si>
   <si>
-    <t>Enc Client Secret</t>
+    <t>Encrypted Client Secret</t>
+  </si>
+  <si>
+    <t>SELECTOR UPDATES</t>
+  </si>
+  <si>
+    <t>Parent Selector</t>
+  </si>
+  <si>
+    <t>&lt;html app='chrome.exe' title='A. P. J. Abdul Kalam: Revision history - Wikipedia' /&gt;</t>
+  </si>
+  <si>
+    <t>Parent Selector for Main Item</t>
+  </si>
+  <si>
+    <t>Child Selector Date</t>
+  </si>
+  <si>
+    <t>&lt;webctrl class='mw-changeslist-date' parentid='pagehistory' tag='A' idx='1' /&gt;</t>
+  </si>
+  <si>
+    <t>Child Selector for Main Date</t>
+  </si>
+  <si>
+    <t>Child Selector Bytes</t>
+  </si>
+  <si>
+    <t>&lt;webctrl parentid='pagehistory' tag='SPAN' class='history-size mw-diff-bytes' idx='1' /&gt;</t>
+  </si>
+  <si>
+    <t>Child Selector for Main Bytes</t>
+  </si>
+  <si>
+    <t>Name_Change</t>
+  </si>
+  <si>
+    <t>20:00, 18 March 2023</t>
+  </si>
+  <si>
+    <t>Size_Change</t>
+  </si>
+  <si>
+    <t>144,909 bytes</t>
+  </si>
+  <si>
+    <t>Automatically updates the Date on which the site was updated</t>
+  </si>
+  <si>
+    <t>Automatically updates the bytes size on which the site was updated</t>
   </si>
 </sst>
 </file>
@@ -148,11 +193,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -160,7 +202,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -500,168 +542,227 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="79.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
         <v>500</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="4" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="C13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>26</v>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>